<commit_message>
Added suppplier's contact info and company twitter
</commit_message>
<xml_diff>
--- a/demo_data/rapid_demo_data.xlsx
+++ b/demo_data/rapid_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NedZhang\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\workspace\s4s\S4S-PerformanceTesting\demo_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959FD6FB-7CB4-4744-A5C7-D7FA06FE6410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D436BF65-FA0A-4428-BFBA-F92226ADACA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="18669" windowHeight="11323" firstSheet="1" activeTab="4" xr2:uid="{55A103A1-F6D8-4E67-9E36-E6481D080608}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" firstSheet="1" activeTab="2" xr2:uid="{55A103A1-F6D8-4E67-9E36-E6481D080608}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Supplier Products" sheetId="4" r:id="rId4"/>
     <sheet name="Supplier Locations" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="186">
   <si>
     <t>Category Name</t>
   </si>
@@ -547,13 +545,61 @@
   </si>
   <si>
     <t>41.991592,-71.491217</t>
+  </si>
+  <si>
+    <t>Contact Person</t>
+  </si>
+  <si>
+    <t>Contact Phone</t>
+  </si>
+  <si>
+    <t>Contact Email</t>
+  </si>
+  <si>
+    <t>Michael D. Hsu</t>
+  </si>
+  <si>
+    <t>1-888-525-8388</t>
+  </si>
+  <si>
+    <t>customerservice@kimberly-clark.com</t>
+  </si>
+  <si>
+    <t>Mike Roman</t>
+  </si>
+  <si>
+    <t>1 954-922-6712</t>
+  </si>
+  <si>
+    <t>help@3m.com</t>
+  </si>
+  <si>
+    <t>Bob Drug</t>
+  </si>
+  <si>
+    <t>1-866-389-2727</t>
+  </si>
+  <si>
+    <t>cvshotline@cvs.com</t>
+  </si>
+  <si>
+    <t>@CVSHealth</t>
+  </si>
+  <si>
+    <t>@3M</t>
+  </si>
+  <si>
+    <t>@KCCorp</t>
+  </si>
+  <si>
+    <t>Company Twitter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,13 +1004,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -972,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -980,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -988,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1010,15 +1056,15 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.15234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.399999999999999">
+    <row r="1" spans="1:4" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1046,7 +1092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1060,7 +1106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1074,7 +1120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1088,7 +1134,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1102,7 +1148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1116,7 +1162,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1130,7 +1176,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1162,28 +1208,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AC9138-2F67-4A69-8066-2BCE4C7E7082}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.3828125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.3828125" customWidth="1"/>
+    <col min="14" max="14" width="22.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1215,10 +1262,22 @@
         <v>42</v>
       </c>
       <c r="K1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M1" t="s">
+        <v>172</v>
+      </c>
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="O1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1249,11 +1308,23 @@
       <c r="J2" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="O2" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1284,11 +1355,23 @@
       <c r="J3" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="O3" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1319,18 +1402,33 @@
       <c r="J4" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
+        <v>179</v>
+      </c>
+      <c r="L4" t="s">
+        <v>180</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{D1873D90-3136-44F0-9CC5-FD7A4BE81015}"/>
-    <hyperlink ref="K3" r:id="rId2" xr:uid="{EB13C02D-1C94-4198-9D20-2FFBBA8DD55D}"/>
-    <hyperlink ref="K4" r:id="rId3" xr:uid="{B6464861-1F50-4523-84DD-201FE6F1EB21}"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{D1873D90-3136-44F0-9CC5-FD7A4BE81015}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{EB13C02D-1C94-4198-9D20-2FFBBA8DD55D}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{B6464861-1F50-4523-84DD-201FE6F1EB21}"/>
+    <hyperlink ref="M2" r:id="rId4" xr:uid="{8A7C8A18-D92E-4449-9CE2-674539774ACC}"/>
+    <hyperlink ref="M3" r:id="rId5" xr:uid="{375B8671-CBF2-41CA-B1AF-D60D2B789431}"/>
+    <hyperlink ref="M4" r:id="rId6" xr:uid="{70B590E2-5018-45FF-B4F9-3DCE0A95AD04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1342,15 +1440,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.69140625" customWidth="1"/>
+    <col min="4" max="4" width="16.15234375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.95">
+    <row r="1" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1370,7 +1468,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1390,7 +1488,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1410,7 +1508,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1430,7 +1528,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1450,7 +1548,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1470,7 +1568,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1490,7 +1588,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1510,7 +1608,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1530,7 +1628,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1550,7 +1648,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1570,7 +1668,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1590,7 +1688,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1610,7 +1708,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1653,21 +1751,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38DABDB6-2B76-47E2-8DCA-025C1DA50497}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.3828125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.95">
+    <row r="1" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>73</v>
       </c>
@@ -1687,7 +1785,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1705,7 +1803,7 @@
         <v>-96.796999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1723,7 +1821,7 @@
         <v>-122.054169</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1741,7 +1839,7 @@
         <v>-118.41</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1759,7 +1857,7 @@
         <v>-122.69</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1777,7 +1875,7 @@
         <v>-117.241112</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1795,7 +1893,7 @@
         <v>-121.85</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1818,7 +1916,7 @@
         <v>-87.0473635</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1841,7 +1939,7 @@
         <v>-87.9014713</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1864,7 +1962,7 @@
         <v>-92.2448031</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1887,7 +1985,7 @@
         <v>-117.5135497</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1910,7 +2008,7 @@
         <v>-117.8450948</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1933,7 +2031,7 @@
         <v>-118.2031029</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1956,7 +2054,7 @@
         <v>-118.5699846</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1979,7 +2077,7 @@
         <v>-75.7005464</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2002,7 +2100,7 @@
         <v>-90.2893936</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2025,7 +2123,7 @@
         <v>-88.7541753</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2048,7 +2146,7 @@
         <v>-85.3586753</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2071,7 +2169,7 @@
         <v>-86.2577368</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -2094,7 +2192,7 @@
         <v>-93.5811265</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2117,7 +2215,7 @@
         <v>-93.0672318</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2140,7 +2238,7 @@
         <v>-84.2967138</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2163,7 +2261,7 @@
         <v>-71.3242059</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -2186,7 +2284,7 @@
         <v>-92.2735209</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -2209,7 +2307,7 @@
         <v>-74.8517819</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -2232,7 +2330,7 @@
         <v>-117.9695004</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -2255,7 +2353,7 @@
         <v>-121.1600557</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -2278,7 +2376,7 @@
         <v>-81.4132831</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2301,7 +2399,7 @@
         <v>-80.534098</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -2324,7 +2422,7 @@
         <v>-86.0633881</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -2500,6 +2598,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2508,20 +2612,37 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08CB37B1-3689-45BC-9694-3471D7F789D0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08CB37B1-3689-45BC-9694-3471D7F789D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f8ac5e7d-7b7d-46e0-8d8a-f4f02b48db66"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B134AECF-465E-46DD-9E1D-992EEFBD7BFD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB559E8-D6DB-47E2-8967-93AEC75CA8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB559E8-D6DB-47E2-8967-93AEC75CA8BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B134AECF-465E-46DD-9E1D-992EEFBD7BFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated with files for setuping up network
</commit_message>
<xml_diff>
--- a/demo_data/rapid_demo_data.xlsx
+++ b/demo_data/rapid_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\workspace\s4s\S4S-PerformanceTesting\demo_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D436BF65-FA0A-4428-BFBA-F92226ADACA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C88706-F5DF-4F50-8D37-1D9C0CE5FD1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" firstSheet="1" activeTab="2" xr2:uid="{55A103A1-F6D8-4E67-9E36-E6481D080608}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8868" activeTab="4" xr2:uid="{55A103A1-F6D8-4E67-9E36-E6481D080608}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="188">
   <si>
     <t>Category Name</t>
   </si>
@@ -593,6 +593,16 @@
   </si>
   <si>
     <t>Company Twitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {
+        "shipNode": "$shipNode",
+        "latitude": $latitude,
+        "longitude": $longitude
+    }</t>
+  </si>
+  <si>
+    <t>JSON for setup</t>
   </si>
 </sst>
 </file>
@@ -673,7 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -683,6 +693,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1004,13 +1017,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1026,7 +1039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1056,15 +1069,15 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.15234375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.45" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1078,7 +1091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1092,7 +1105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1106,7 +1119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1120,7 +1133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1134,7 +1147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1148,7 +1161,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1162,7 +1175,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1176,7 +1189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1210,27 +1223,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AC9138-2F67-4A69-8066-2BCE4C7E7082}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.15234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.15234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.3828125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="13.3828125" customWidth="1"/>
-    <col min="14" max="14" width="22.53515625" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1277,7 +1289,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1371,7 +1383,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1440,15 +1452,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.69140625" customWidth="1"/>
-    <col min="4" max="4" width="16.15234375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1468,7 +1480,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1488,7 +1500,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1528,7 +1540,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1548,7 +1560,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1568,7 +1580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1608,7 +1620,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1648,7 +1660,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1668,7 +1680,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1688,7 +1700,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1708,7 +1720,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1749,23 +1761,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38DABDB6-2B76-47E2-8DCA-025C1DA50497}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>73</v>
       </c>
@@ -1784,8 +1797,14 @@
       <c r="F1" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1802,8 +1821,17 @@
       <c r="F2" s="6">
         <v>-96.796999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G2" s="6"/>
+      <c r="H2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE( SUBSTITUTE($K$1, "$shipNode", _xlfn.CONCAT(A2, "::", B2)), "$latitude", E2), "$longitude", F2)</f>
+        <v xml:space="preserve">  {
+        "shipNode": "KC::DALLAS",
+        "latitude": 32.7767,
+        "longitude": -96.797
+    }</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1820,8 +1848,17 @@
       <c r="F3" s="6">
         <v>-122.054169</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G3" s="6"/>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H31" si="0">SUBSTITUTE(SUBSTITUTE( SUBSTITUTE($K$1, "$shipNode", _xlfn.CONCAT(A3, "::", B3)), "$latitude", E3), "$longitude", F3)</f>
+        <v xml:space="preserve">  {
+        "shipNode": "KC::FAIRFIELD",
+        "latitude": 38.2577781,
+        "longitude": -122.054169
+    }</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1838,8 +1875,17 @@
       <c r="F4" s="6">
         <v>-118.41</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G4" s="6"/>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "KC::LOSANGELES",
+        "latitude": 34.11,
+        "longitude": -118.41
+    }</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1856,8 +1902,17 @@
       <c r="F5" s="6">
         <v>-122.69</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G5" s="6"/>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "KC::SANFRANCISCO",
+        "latitude": 37.76,
+        "longitude": -122.69
+    }</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1874,8 +1929,17 @@
       <c r="F6" s="6">
         <v>-117.241112</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G6" s="6"/>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "KC::VISTA",
+        "latitude": 33.193611,
+        "longitude": -117.241112
+    }</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1892,8 +1956,17 @@
       <c r="F7" s="6">
         <v>-121.85</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G7" s="6"/>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "KC::SANJOSE",
+        "latitude": 37.3,
+        "longitude": -121.85
+    }</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1915,8 +1988,16 @@
         <f>RIGHT(D8, LEN(D8)- SEARCH(",", D8))</f>
         <v>-87.0473635</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Decatur",
+        "latitude": 34.6422621,
+        "longitude": -87.0473635
+    }</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1924,7 +2005,7 @@
         <v>124</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" ref="C9:C24" si="0">_xlfn.CONCAT(A9, " ", B9, " plant")</f>
+        <f t="shared" ref="C9:C24" si="1">_xlfn.CONCAT(A9, " ", B9, " plant")</f>
         <v>3M Guin plant</v>
       </c>
       <c r="D9" t="s">
@@ -1938,8 +2019,16 @@
         <f>RIGHT(D9, LEN(D9)- SEARCH(",", D9))</f>
         <v>-87.9014713</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Guin",
+        "latitude": 33.9674381,
+        "longitude": -87.9014713
+    }</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1947,22 +2036,30 @@
         <v>126</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Little Rock plant</v>
       </c>
       <c r="D10" t="s">
         <v>127</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" ref="E10:E31" si="1">LEFT(D10, SEARCH(",", D10)-1)</f>
+        <f t="shared" ref="E10:E31" si="2">LEFT(D10, SEARCH(",", D10)-1)</f>
         <v>34.707139</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" ref="F10:F24" si="2">RIGHT(D10, LEN(D10)- SEARCH(",", D10))</f>
+        <f t="shared" ref="F10:F24" si="3">RIGHT(D10, LEN(D10)- SEARCH(",", D10))</f>
         <v>-92.2448031</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Little Rock",
+        "latitude": 34.707139,
+        "longitude": -92.2448031
+    }</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1970,22 +2067,30 @@
         <v>128</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Corona plant</v>
       </c>
       <c r="D11" t="s">
         <v>129</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.8461148</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-117.5135497</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Corona",
+        "latitude": 33.8461148,
+        "longitude": -117.5135497
+    }</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1993,22 +2098,30 @@
         <v>130</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Irvine plant</v>
       </c>
       <c r="D12" t="s">
         <v>131</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.6926525</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-117.8450948</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Irvine",
+        "latitude": 33.6926525,
+        "longitude": -117.8450948
+    }</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2016,22 +2129,30 @@
         <v>132</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Monrovia plant</v>
       </c>
       <c r="D13" t="s">
         <v>133</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.912692</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-118.2031029</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Monrovia",
+        "latitude": 33.912692,
+        "longitude": -118.2031029
+    }</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -2039,22 +2160,30 @@
         <v>134</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Northridge plant</v>
       </c>
       <c r="D14" t="s">
         <v>135</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.233492</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-118.5699846</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Northridge",
+        "latitude": 34.233492,
+        "longitude": -118.5699846
+    }</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2062,22 +2191,30 @@
         <v>136</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Newark plant</v>
       </c>
       <c r="D15" t="s">
         <v>137</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39.9320396</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-75.7005464</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Newark",
+        "latitude": 39.9320396,
+        "longitude": -75.7005464
+    }</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2085,22 +2222,30 @@
         <v>138</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Cordova plant</v>
       </c>
       <c r="D16" t="s">
         <v>139</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41.7520093</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-90.2893936</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Cordova",
+        "latitude": 41.7520093,
+        "longitude": -90.2893936
+    }</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2108,22 +2253,30 @@
         <v>140</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M DeKalb plant</v>
       </c>
       <c r="D17" t="s">
         <v>141</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41.9038735</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-88.7541753</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::DeKalb",
+        "latitude": 41.9038735,
+        "longitude": -88.7541753
+    }</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2131,22 +2284,30 @@
         <v>142</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Hartford City plant</v>
       </c>
       <c r="D18" t="s">
         <v>143</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40.445837</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-85.3586753</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Hartford City",
+        "latitude": 40.445837,
+        "longitude": -85.3586753
+    }</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2154,22 +2315,30 @@
         <v>144</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Indianapolis plant</v>
       </c>
       <c r="D19" t="s">
         <v>145</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39.8961877</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-86.2577368</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Indianapolis",
+        "latitude": 39.8961877,
+        "longitude": -86.2577368
+    }</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -2177,22 +2346,30 @@
         <v>146</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Ames plant</v>
       </c>
       <c r="D20" t="s">
         <v>147</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42.0296479</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-93.5811265</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Ames",
+        "latitude": 42.0296479,
+        "longitude": -93.5811265
+    }</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2200,22 +2377,30 @@
         <v>148</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Knoxville plant</v>
       </c>
       <c r="D21" t="s">
         <v>149</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41.3199819</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-93.0672318</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Knoxville",
+        "latitude": 41.3199819,
+        "longitude": -93.0672318
+    }</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2223,22 +2408,30 @@
         <v>150</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Cynthiana plant</v>
       </c>
       <c r="D22" t="s">
         <v>151</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38.3736534</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-84.2967138</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Cynthiana",
+        "latitude": 38.3736534,
+        "longitude": -84.2967138
+    }</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2246,22 +2439,30 @@
         <v>152</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Chelmsford plant</v>
       </c>
       <c r="D23" t="s">
         <v>153</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42.5945467</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-71.3242059</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Chelmsford",
+        "latitude": 42.5945467,
+        "longitude": -71.3242059
+    }</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -2269,22 +2470,30 @@
         <v>154</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3M Columbia plant</v>
       </c>
       <c r="D24" t="s">
         <v>155</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39.0097514</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-92.2735209</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "3M::Columbia",
+        "latitude": 39.0097514,
+        "longitude": -92.2735209
+    }</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -2299,15 +2508,23 @@
         <v>157</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39.9873935</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" ref="F25" si="3">RIGHT(D25, LEN(D25)- SEARCH(",", D25))</f>
+        <f t="shared" ref="F25" si="4">RIGHT(D25, LEN(D25)- SEARCH(",", D25))</f>
         <v>-74.8517819</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "CVS::NJ Lumberton",
+        "latitude": 39.9873935,
+        "longitude": -74.8517819
+    }</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -2315,22 +2532,30 @@
         <v>158</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" ref="C26:C31" si="4">_xlfn.CONCAT(A26, " ", B26, " Distribution center")</f>
+        <f t="shared" ref="C26:C31" si="5">_xlfn.CONCAT(A26, " ", B26, " Distribution center")</f>
         <v>CVS CA - La Habra Distribution center</v>
       </c>
       <c r="D26" t="s">
         <v>159</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.0471555</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" ref="F26:F31" si="5">RIGHT(D26, LEN(D26)- SEARCH(",", D26))</f>
+        <f t="shared" ref="F26:F31" si="6">RIGHT(D26, LEN(D26)- SEARCH(",", D26))</f>
         <v>-117.9695004</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "CVS::CA - La Habra",
+        "latitude": 34.0471555,
+        "longitude": -117.9695004
+    }</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -2338,22 +2563,30 @@
         <v>160</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CVS CA - Patterson Distribution center</v>
       </c>
       <c r="D27" t="s">
         <v>161</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37.4692705</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-121.1600557</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "CVS::CA - Patterson",
+        "latitude": 37.4692705,
+        "longitude": -121.1600557
+    }</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -2361,22 +2594,30 @@
         <v>162</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CVS FL - Orlando Distribution center</v>
       </c>
       <c r="D28" t="s">
         <v>163</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.4443035</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-81.4132831</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "CVS::FL - Orlando",
+        "latitude": 28.4443035,
+        "longitude": -81.4132831
+    }</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2384,22 +2625,30 @@
         <v>164</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CVS FL - Vero Beach Distribution center</v>
       </c>
       <c r="D29" t="s">
         <v>165</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27.6449214</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-80.534098</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "CVS::FL - Vero Beach",
+        "latitude": 27.6449214,
+        "longitude": -80.534098
+    }</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -2407,22 +2656,30 @@
         <v>166</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CVS IN - Indianapolis Distribution center</v>
       </c>
       <c r="D30" t="s">
         <v>167</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39.8006766</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-86.0633881</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "CVS::IN - Indianapolis",
+        "latitude": 39.8006766,
+        "longitude": -86.0633881
+    }</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -2430,19 +2687,27 @@
         <v>168</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CVS RI - Woonsocket Distribution center</v>
       </c>
       <c r="D31" t="s">
         <v>169</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41.991592</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-71.491217</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  {
+        "shipNode": "CVS::RI - Woonsocket",
+        "latitude": 41.991592,
+        "longitude": -71.491217
+    }</v>
       </c>
     </row>
   </sheetData>
@@ -2452,6 +2717,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0FB48E7781CB14ABDFC5701083D6948" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ae3a81944bad549e169a2298e75529d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f8ac5e7d-7b7d-46e0-8d8a-f4f02b48db66" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9b295d8d52636200d9ed62a0a1a9ab6" ns3:_="">
     <xsd:import namespace="f8ac5e7d-7b7d-46e0-8d8a-f4f02b48db66"/>
@@ -2597,22 +2877,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B134AECF-465E-46DD-9E1D-992EEFBD7BFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB559E8-D6DB-47E2-8967-93AEC75CA8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08CB37B1-3689-45BC-9694-3471D7F789D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2628,21 +2910,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB559E8-D6DB-47E2-8967-93AEC75CA8BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B134AECF-465E-46DD-9E1D-992EEFBD7BFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added script for loading suppplier locations and item relationship
</commit_message>
<xml_diff>
--- a/demo_data/rapid_demo_data.xlsx
+++ b/demo_data/rapid_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\workspace\s4s\S4S-PerformanceTesting\demo_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C88706-F5DF-4F50-8D37-1D9C0CE5FD1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94565B32-D1F2-4276-9ACC-344A1B5156A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8868" activeTab="4" xr2:uid="{55A103A1-F6D8-4E67-9E36-E6481D080608}"/>
+    <workbookView xWindow="1474" yWindow="1474" windowWidth="24686" windowHeight="13192" activeTab="4" xr2:uid="{55A103A1-F6D8-4E67-9E36-E6481D080608}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="186">
   <si>
     <t>Category Name</t>
   </si>
@@ -593,16 +593,6 @@
   </si>
   <si>
     <t>Company Twitter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  {
-        "shipNode": "$shipNode",
-        "latitude": $latitude,
-        "longitude": $longitude
-    }</t>
-  </si>
-  <si>
-    <t>JSON for setup</t>
   </si>
 </sst>
 </file>
@@ -683,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -693,9 +683,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1017,13 +1004,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1069,15 +1056,15 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1091,7 +1078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1119,7 +1106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1133,7 +1120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1147,7 +1134,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1162,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1189,7 +1176,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1227,22 +1214,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.07421875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.3046875" customWidth="1"/>
+    <col min="14" max="14" width="22.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1289,7 +1276,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1336,7 +1323,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1383,7 +1370,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1452,15 +1439,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.69140625" customWidth="1"/>
+    <col min="4" max="4" width="16.07421875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1480,7 +1467,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1500,7 +1487,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1520,7 +1507,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1540,7 +1527,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1560,7 +1547,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1580,7 +1567,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1600,7 +1587,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1620,7 +1607,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1640,7 +1627,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1660,7 +1647,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1680,7 +1667,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1700,7 +1687,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1707,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1761,24 +1748,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38DABDB6-2B76-47E2-8DCA-025C1DA50497}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.3046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>73</v>
       </c>
@@ -1797,14 +1784,8 @@
       <c r="F1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1821,17 +1802,8 @@
       <c r="F2" s="6">
         <v>-96.796999999999997</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE( SUBSTITUTE($K$1, "$shipNode", _xlfn.CONCAT(A2, "::", B2)), "$latitude", E2), "$longitude", F2)</f>
-        <v xml:space="preserve">  {
-        "shipNode": "KC::DALLAS",
-        "latitude": 32.7767,
-        "longitude": -96.797
-    }</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1848,17 +1820,8 @@
       <c r="F3" s="6">
         <v>-122.054169</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H31" si="0">SUBSTITUTE(SUBSTITUTE( SUBSTITUTE($K$1, "$shipNode", _xlfn.CONCAT(A3, "::", B3)), "$latitude", E3), "$longitude", F3)</f>
-        <v xml:space="preserve">  {
-        "shipNode": "KC::FAIRFIELD",
-        "latitude": 38.2577781,
-        "longitude": -122.054169
-    }</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1875,17 +1838,8 @@
       <c r="F4" s="6">
         <v>-118.41</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "KC::LOSANGELES",
-        "latitude": 34.11,
-        "longitude": -118.41
-    }</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1902,17 +1856,8 @@
       <c r="F5" s="6">
         <v>-122.69</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "KC::SANFRANCISCO",
-        "latitude": 37.76,
-        "longitude": -122.69
-    }</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1929,17 +1874,8 @@
       <c r="F6" s="6">
         <v>-117.241112</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "KC::VISTA",
-        "latitude": 33.193611,
-        "longitude": -117.241112
-    }</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1956,17 +1892,8 @@
       <c r="F7" s="6">
         <v>-121.85</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "KC::SANJOSE",
-        "latitude": 37.3,
-        "longitude": -121.85
-    }</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1988,16 +1915,8 @@
         <f>RIGHT(D8, LEN(D8)- SEARCH(",", D8))</f>
         <v>-87.0473635</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Decatur",
-        "latitude": 34.6422621,
-        "longitude": -87.0473635
-    }</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2005,7 +1924,7 @@
         <v>124</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" ref="C9:C24" si="1">_xlfn.CONCAT(A9, " ", B9, " plant")</f>
+        <f t="shared" ref="C9:C24" si="0">_xlfn.CONCAT(A9, " ", B9, " plant")</f>
         <v>3M Guin plant</v>
       </c>
       <c r="D9" t="s">
@@ -2019,16 +1938,8 @@
         <f>RIGHT(D9, LEN(D9)- SEARCH(",", D9))</f>
         <v>-87.9014713</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Guin",
-        "latitude": 33.9674381,
-        "longitude": -87.9014713
-    }</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2036,30 +1947,22 @@
         <v>126</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Little Rock plant</v>
       </c>
       <c r="D10" t="s">
         <v>127</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" ref="E10:E31" si="2">LEFT(D10, SEARCH(",", D10)-1)</f>
+        <f t="shared" ref="E10:E31" si="1">LEFT(D10, SEARCH(",", D10)-1)</f>
         <v>34.707139</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" ref="F10:F24" si="3">RIGHT(D10, LEN(D10)- SEARCH(",", D10))</f>
+        <f t="shared" ref="F10:F24" si="2">RIGHT(D10, LEN(D10)- SEARCH(",", D10))</f>
         <v>-92.2448031</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Little Rock",
-        "latitude": 34.707139,
-        "longitude": -92.2448031
-    }</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -2067,30 +1970,22 @@
         <v>128</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Corona plant</v>
       </c>
       <c r="D11" t="s">
         <v>129</v>
       </c>
       <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>33.8461148</v>
+      </c>
+      <c r="F11" t="str">
         <f t="shared" si="2"/>
-        <v>33.8461148</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="3"/>
         <v>-117.5135497</v>
       </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Corona",
-        "latitude": 33.8461148,
-        "longitude": -117.5135497
-    }</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2098,30 +1993,22 @@
         <v>130</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Irvine plant</v>
       </c>
       <c r="D12" t="s">
         <v>131</v>
       </c>
       <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>33.6926525</v>
+      </c>
+      <c r="F12" t="str">
         <f t="shared" si="2"/>
-        <v>33.6926525</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="3"/>
         <v>-117.8450948</v>
       </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Irvine",
-        "latitude": 33.6926525,
-        "longitude": -117.8450948
-    }</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2129,30 +2016,22 @@
         <v>132</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Monrovia plant</v>
       </c>
       <c r="D13" t="s">
         <v>133</v>
       </c>
       <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>33.912692</v>
+      </c>
+      <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v>33.912692</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="3"/>
         <v>-118.2031029</v>
       </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Monrovia",
-        "latitude": 33.912692,
-        "longitude": -118.2031029
-    }</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -2160,30 +2039,22 @@
         <v>134</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Northridge plant</v>
       </c>
       <c r="D14" t="s">
         <v>135</v>
       </c>
       <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>34.233492</v>
+      </c>
+      <c r="F14" t="str">
         <f t="shared" si="2"/>
-        <v>34.233492</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="3"/>
         <v>-118.5699846</v>
       </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Northridge",
-        "latitude": 34.233492,
-        "longitude": -118.5699846
-    }</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2191,30 +2062,22 @@
         <v>136</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Newark plant</v>
       </c>
       <c r="D15" t="s">
         <v>137</v>
       </c>
       <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>39.9320396</v>
+      </c>
+      <c r="F15" t="str">
         <f t="shared" si="2"/>
-        <v>39.9320396</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="3"/>
         <v>-75.7005464</v>
       </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Newark",
-        "latitude": 39.9320396,
-        "longitude": -75.7005464
-    }</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2222,30 +2085,22 @@
         <v>138</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Cordova plant</v>
       </c>
       <c r="D16" t="s">
         <v>139</v>
       </c>
       <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>41.7520093</v>
+      </c>
+      <c r="F16" t="str">
         <f t="shared" si="2"/>
-        <v>41.7520093</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="3"/>
         <v>-90.2893936</v>
       </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Cordova",
-        "latitude": 41.7520093,
-        "longitude": -90.2893936
-    }</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2253,30 +2108,22 @@
         <v>140</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M DeKalb plant</v>
       </c>
       <c r="D17" t="s">
         <v>141</v>
       </c>
       <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>41.9038735</v>
+      </c>
+      <c r="F17" t="str">
         <f t="shared" si="2"/>
-        <v>41.9038735</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="3"/>
         <v>-88.7541753</v>
       </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::DeKalb",
-        "latitude": 41.9038735,
-        "longitude": -88.7541753
-    }</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2284,30 +2131,22 @@
         <v>142</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Hartford City plant</v>
       </c>
       <c r="D18" t="s">
         <v>143</v>
       </c>
       <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>40.445837</v>
+      </c>
+      <c r="F18" t="str">
         <f t="shared" si="2"/>
-        <v>40.445837</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="3"/>
         <v>-85.3586753</v>
       </c>
-      <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Hartford City",
-        "latitude": 40.445837,
-        "longitude": -85.3586753
-    }</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2315,30 +2154,22 @@
         <v>144</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Indianapolis plant</v>
       </c>
       <c r="D19" t="s">
         <v>145</v>
       </c>
       <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>39.8961877</v>
+      </c>
+      <c r="F19" t="str">
         <f t="shared" si="2"/>
-        <v>39.8961877</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="3"/>
         <v>-86.2577368</v>
       </c>
-      <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Indianapolis",
-        "latitude": 39.8961877,
-        "longitude": -86.2577368
-    }</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -2346,30 +2177,22 @@
         <v>146</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Ames plant</v>
       </c>
       <c r="D20" t="s">
         <v>147</v>
       </c>
       <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>42.0296479</v>
+      </c>
+      <c r="F20" t="str">
         <f t="shared" si="2"/>
-        <v>42.0296479</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="3"/>
         <v>-93.5811265</v>
       </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Ames",
-        "latitude": 42.0296479,
-        "longitude": -93.5811265
-    }</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2377,30 +2200,22 @@
         <v>148</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Knoxville plant</v>
       </c>
       <c r="D21" t="s">
         <v>149</v>
       </c>
       <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>41.3199819</v>
+      </c>
+      <c r="F21" t="str">
         <f t="shared" si="2"/>
-        <v>41.3199819</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="3"/>
         <v>-93.0672318</v>
       </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Knoxville",
-        "latitude": 41.3199819,
-        "longitude": -93.0672318
-    }</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2408,30 +2223,22 @@
         <v>150</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Cynthiana plant</v>
       </c>
       <c r="D22" t="s">
         <v>151</v>
       </c>
       <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>38.3736534</v>
+      </c>
+      <c r="F22" t="str">
         <f t="shared" si="2"/>
-        <v>38.3736534</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="3"/>
         <v>-84.2967138</v>
       </c>
-      <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Cynthiana",
-        "latitude": 38.3736534,
-        "longitude": -84.2967138
-    }</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2439,30 +2246,22 @@
         <v>152</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Chelmsford plant</v>
       </c>
       <c r="D23" t="s">
         <v>153</v>
       </c>
       <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>42.5945467</v>
+      </c>
+      <c r="F23" t="str">
         <f t="shared" si="2"/>
-        <v>42.5945467</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="3"/>
         <v>-71.3242059</v>
       </c>
-      <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Chelmsford",
-        "latitude": 42.5945467,
-        "longitude": -71.3242059
-    }</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -2470,30 +2269,22 @@
         <v>154</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3M Columbia plant</v>
       </c>
       <c r="D24" t="s">
         <v>155</v>
       </c>
       <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>39.0097514</v>
+      </c>
+      <c r="F24" t="str">
         <f t="shared" si="2"/>
-        <v>39.0097514</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="3"/>
         <v>-92.2735209</v>
       </c>
-      <c r="H24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "3M::Columbia",
-        "latitude": 39.0097514,
-        "longitude": -92.2735209
-    }</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -2508,23 +2299,15 @@
         <v>157</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>39.9873935</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" ref="F25" si="4">RIGHT(D25, LEN(D25)- SEARCH(",", D25))</f>
+        <f t="shared" ref="F25" si="3">RIGHT(D25, LEN(D25)- SEARCH(",", D25))</f>
         <v>-74.8517819</v>
       </c>
-      <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "CVS::NJ Lumberton",
-        "latitude": 39.9873935,
-        "longitude": -74.8517819
-    }</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -2532,30 +2315,22 @@
         <v>158</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" ref="C26:C31" si="5">_xlfn.CONCAT(A26, " ", B26, " Distribution center")</f>
+        <f t="shared" ref="C26:C31" si="4">_xlfn.CONCAT(A26, " ", B26, " Distribution center")</f>
         <v>CVS CA - La Habra Distribution center</v>
       </c>
       <c r="D26" t="s">
         <v>159</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>34.0471555</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" ref="F26:F31" si="6">RIGHT(D26, LEN(D26)- SEARCH(",", D26))</f>
+        <f t="shared" ref="F26:F31" si="5">RIGHT(D26, LEN(D26)- SEARCH(",", D26))</f>
         <v>-117.9695004</v>
       </c>
-      <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "CVS::CA - La Habra",
-        "latitude": 34.0471555,
-        "longitude": -117.9695004
-    }</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -2563,30 +2338,22 @@
         <v>160</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>CVS CA - Patterson Distribution center</v>
       </c>
       <c r="D27" t="s">
         <v>161</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>37.4692705</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-121.1600557</v>
       </c>
-      <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "CVS::CA - Patterson",
-        "latitude": 37.4692705,
-        "longitude": -121.1600557
-    }</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -2594,30 +2361,22 @@
         <v>162</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>CVS FL - Orlando Distribution center</v>
       </c>
       <c r="D28" t="s">
         <v>163</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>28.4443035</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-81.4132831</v>
       </c>
-      <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "CVS::FL - Orlando",
-        "latitude": 28.4443035,
-        "longitude": -81.4132831
-    }</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2625,30 +2384,22 @@
         <v>164</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>CVS FL - Vero Beach Distribution center</v>
       </c>
       <c r="D29" t="s">
         <v>165</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27.6449214</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-80.534098</v>
       </c>
-      <c r="H29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "CVS::FL - Vero Beach",
-        "latitude": 27.6449214,
-        "longitude": -80.534098
-    }</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -2656,30 +2407,22 @@
         <v>166</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>CVS IN - Indianapolis Distribution center</v>
       </c>
       <c r="D30" t="s">
         <v>167</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>39.8006766</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-86.0633881</v>
       </c>
-      <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "CVS::IN - Indianapolis",
-        "latitude": 39.8006766,
-        "longitude": -86.0633881
-    }</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -2687,27 +2430,19 @@
         <v>168</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>CVS RI - Woonsocket Distribution center</v>
       </c>
       <c r="D31" t="s">
         <v>169</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>41.991592</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-71.491217</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  {
-        "shipNode": "CVS::RI - Woonsocket",
-        "latitude": 41.991592,
-        "longitude": -71.491217
-    }</v>
       </c>
     </row>
   </sheetData>
@@ -2717,21 +2452,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0FB48E7781CB14ABDFC5701083D6948" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ae3a81944bad549e169a2298e75529d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f8ac5e7d-7b7d-46e0-8d8a-f4f02b48db66" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9b295d8d52636200d9ed62a0a1a9ab6" ns3:_="">
     <xsd:import namespace="f8ac5e7d-7b7d-46e0-8d8a-f4f02b48db66"/>
@@ -2877,24 +2597,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B134AECF-465E-46DD-9E1D-992EEFBD7BFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB559E8-D6DB-47E2-8967-93AEC75CA8BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08CB37B1-3689-45BC-9694-3471D7F789D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2910,4 +2628,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB559E8-D6DB-47E2-8967-93AEC75CA8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B134AECF-465E-46DD-9E1D-992EEFBD7BFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
reset 3m file and updated to the upload ipynb
</commit_message>
<xml_diff>
--- a/demo_data/rapid_demo_data.xlsx
+++ b/demo_data/rapid_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\workspace\s4s\S4S-PerformanceTesting\demo_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94565B32-D1F2-4276-9ACC-344A1B5156A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BDF23D-3B8B-4B1C-B459-AAC9D0DA8B35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1474" yWindow="1474" windowWidth="24686" windowHeight="13192" activeTab="4" xr2:uid="{55A103A1-F6D8-4E67-9E36-E6481D080608}"/>
+    <workbookView xWindow="1474" yWindow="1474" windowWidth="22132" windowHeight="13192" activeTab="3" xr2:uid="{55A103A1-F6D8-4E67-9E36-E6481D080608}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="2" r:id="rId1"/>
@@ -340,9 +340,6 @@
     <t>https://multimedia.3m.com/mws/media/811728P/3mtm-auratm-particulate-respirator-9211-plus-n95.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">399575 </t>
-  </si>
-  <si>
     <t>CVS Health Procedural Face Masks With Earloops</t>
   </si>
   <si>
@@ -593,6 +590,9 @@
   </si>
   <si>
     <t>Company Twitter</t>
+  </si>
+  <si>
+    <t>399575</t>
   </si>
 </sst>
 </file>
@@ -1261,19 +1261,19 @@
         <v>42</v>
       </c>
       <c r="K1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" t="s">
         <v>170</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>171</v>
-      </c>
-      <c r="M1" t="s">
-        <v>172</v>
       </c>
       <c r="N1" t="s">
         <v>43</v>
       </c>
       <c r="O1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
@@ -1308,19 +1308,19 @@
         <v>51</v>
       </c>
       <c r="K2" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" t="s">
         <v>173</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
@@ -1355,19 +1355,19 @@
         <v>60</v>
       </c>
       <c r="K3" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" t="s">
         <v>176</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
@@ -1402,19 +1402,19 @@
         <v>70</v>
       </c>
       <c r="K4" t="s">
+        <v>178</v>
+      </c>
+      <c r="L4" t="s">
         <v>179</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1435,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E572313C-35E0-4CE1-8C53-1EB322ECC5AA}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1698,13 +1698,13 @@
         <v>62</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" t="s">
         <v>101</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
@@ -1718,10 +1718,10 @@
         <v>62</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" t="s">
         <v>104</v>
-      </c>
-      <c r="E14" t="s">
-        <v>105</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>100</v>
@@ -1750,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38DABDB6-2B76-47E2-8DCA-025C1DA50497}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1770,19 +1770,19 @@
         <v>73</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1790,10 +1790,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6">
@@ -1808,10 +1808,10 @@
         <v>44</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6">
@@ -1826,10 +1826,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>115</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6">
@@ -1844,10 +1844,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6">
@@ -1862,10 +1862,10 @@
         <v>44</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6">
@@ -1880,10 +1880,10 @@
         <v>44</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
@@ -1898,14 +1898,14 @@
         <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(A8, " ", B8, " plant")</f>
         <v>3M Decatur plant</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" t="str">
         <f>LEFT(D8, SEARCH(",", D8)-1)</f>
@@ -1921,14 +1921,14 @@
         <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" ref="C9:C24" si="0">_xlfn.CONCAT(A9, " ", B9, " plant")</f>
         <v>3M Guin plant</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" t="str">
         <f>LEFT(D9, SEARCH(",", D9)-1)</f>
@@ -1944,14 +1944,14 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>3M Little Rock plant</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" ref="E10:E31" si="1">LEFT(D10, SEARCH(",", D10)-1)</f>
@@ -1967,14 +1967,14 @@
         <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>3M Corona plant</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
@@ -1990,14 +1990,14 @@
         <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>3M Irvine plant</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
@@ -2013,14 +2013,14 @@
         <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>3M Monrovia plant</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
@@ -2036,14 +2036,14 @@
         <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>3M Northridge plant</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
@@ -2059,14 +2059,14 @@
         <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>3M Newark plant</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
@@ -2082,14 +2082,14 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>3M Cordova plant</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
@@ -2105,14 +2105,14 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>3M DeKalb plant</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
@@ -2128,14 +2128,14 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>3M Hartford City plant</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
@@ -2151,14 +2151,14 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>3M Indianapolis plant</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
@@ -2174,14 +2174,14 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>3M Ames plant</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
@@ -2197,14 +2197,14 @@
         <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>3M Knoxville plant</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
@@ -2220,14 +2220,14 @@
         <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>3M Cynthiana plant</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
@@ -2243,14 +2243,14 @@
         <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>3M Chelmsford plant</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
@@ -2266,14 +2266,14 @@
         <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>3M Columbia plant</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
@@ -2289,14 +2289,14 @@
         <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.CONCAT(A25, " ", B25, " Distribution center")</f>
         <v>CVS NJ Lumberton Distribution center</v>
       </c>
       <c r="D25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
@@ -2312,14 +2312,14 @@
         <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" ref="C26:C31" si="4">_xlfn.CONCAT(A26, " ", B26, " Distribution center")</f>
         <v>CVS CA - La Habra Distribution center</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
@@ -2335,14 +2335,14 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="4"/>
         <v>CVS CA - Patterson Distribution center</v>
       </c>
       <c r="D27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
@@ -2358,14 +2358,14 @@
         <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="4"/>
         <v>CVS FL - Orlando Distribution center</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
@@ -2381,14 +2381,14 @@
         <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="4"/>
         <v>CVS FL - Vero Beach Distribution center</v>
       </c>
       <c r="D29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
@@ -2404,14 +2404,14 @@
         <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="4"/>
         <v>CVS IN - Indianapolis Distribution center</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
@@ -2427,14 +2427,14 @@
         <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="4"/>
         <v>CVS RI - Woonsocket Distribution center</v>
       </c>
       <c r="D31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
@@ -2452,6 +2452,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0FB48E7781CB14ABDFC5701083D6948" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ae3a81944bad549e169a2298e75529d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f8ac5e7d-7b7d-46e0-8d8a-f4f02b48db66" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9b295d8d52636200d9ed62a0a1a9ab6" ns3:_="">
     <xsd:import namespace="f8ac5e7d-7b7d-46e0-8d8a-f4f02b48db66"/>
@@ -2597,22 +2612,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B134AECF-465E-46DD-9E1D-992EEFBD7BFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB559E8-D6DB-47E2-8967-93AEC75CA8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08CB37B1-3689-45BC-9694-3471D7F789D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2628,21 +2645,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB559E8-D6DB-47E2-8967-93AEC75CA8BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B134AECF-465E-46DD-9E1D-992EEFBD7BFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>